<commit_message>
🔄 Actualización automática de datos
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/ingestion.xlsx
+++ b/src/bigdata/static/xlsx/ingestion.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-03-01 03:15:25</t>
+          <t>2025-03-01 03:18:25</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización Automática de Datos y Limpieza ✅🎉
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/ingestion.xlsx
+++ b/src/bigdata/static/xlsx/ingestion.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-03-07 20:27:45</t>
+          <t>2025-03-07 20:35:20</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualización Automática de Datos (EA1) y (EA2) ✅🎉
</commit_message>
<xml_diff>
--- a/src/bigdata/static/xlsx/ingestion.xlsx
+++ b/src/bigdata/static/xlsx/ingestion.xlsx
@@ -499,7 +499,7 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -527,7 +527,7 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -555,7 +555,7 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -583,7 +583,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -639,7 +639,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -695,7 +695,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -751,7 +751,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -807,7 +807,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -863,7 +863,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -919,7 +919,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -975,7 +975,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1143,7 +1143,7 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1255,7 +1255,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1283,7 +1283,7 @@
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1311,7 +1311,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1339,7 +1339,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1395,7 +1395,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1423,7 +1423,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1535,7 +1535,7 @@
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1591,7 +1591,7 @@
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1647,7 +1647,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1675,7 +1675,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1703,7 +1703,7 @@
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1759,7 +1759,7 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1787,7 +1787,7 @@
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>2025-03-07 20:35:20</t>
+          <t>2025-03-14 03:54:41</t>
         </is>
       </c>
     </row>

</xml_diff>